<commit_message>
Purchase Order Flow- Added Other Deatils and Line Deatils and Comments
</commit_message>
<xml_diff>
--- a/Data Files/TestResult.xlsx
+++ b/Data Files/TestResult.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t/>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>SUCCESFUL:Naviagted To SalesOrder Page</t>
   </si>
 </sst>
 </file>
@@ -105,17 +102,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>